<commit_message>
AUTOMATE-7: Add patient functionality
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CC2327D-853E-4E52-8085-7A1D1F89329E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F7D5B96-B860-4175-9BB8-DE207C9A1C38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="240" yWindow="480" windowWidth="21600" windowHeight="11295" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -2089,7 +2089,7 @@
       </c>
       <c r="E1" s="25" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C993), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C993))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 10 PERCENT = 0%</v>
+        <v>UPDATE = 1 OUT OF 10 PERCENT = 10%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2101,7 +2101,7 @@
         <v>90</v>
       </c>
       <c r="C2" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="28"/>
     </row>

</xml_diff>

<commit_message>
Update logic for saving result
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F713DEE-2727-4FB2-9D58-2F90799011EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9381C3-666F-43C7-BC1C-86ECCF7A1CC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="1485" windowWidth="21600" windowHeight="11235" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1113,26 +1113,6 @@
       <t xml:space="preserve">
 Scenario &amp; Failure Explanation</t>
     </r>
-  </si>
-  <si>
-    <t>•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1
-•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1
-•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1
-•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1
-•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1
-•Added guardian validation 
-     •Expected output: Total Found: 1
-     •Actual Output: Total Found: 1</t>
   </si>
 </sst>
 </file>
@@ -2082,7 +2062,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2113,7 +2093,7 @@
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="270.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -2123,9 +2103,7 @@
       <c r="C2" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="28" t="s">
-        <v>93</v>
-      </c>
+      <c r="D2" s="28"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
Update feed result logic
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC5181D-70EA-41CB-B3C0-4A43CF9BE60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C0248E-C428-4FA6-89A2-53CFDE39768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -2065,7 +2065,7 @@
   <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="E1" s="25" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C993), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C993))*100,2), "%")</f>
-        <v>UPDATE = 2 OUT OF 10 PERCENT = 20%</v>
+        <v>UPDATE = 0 OUT OF 10 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2169,7 +2169,7 @@
         <v>90</v>
       </c>
       <c r="C8" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="28"/>
     </row>
@@ -2181,7 +2181,7 @@
         <v>91</v>
       </c>
       <c r="C9" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="28"/>
     </row>
@@ -2195,6 +2195,7 @@
       <c r="C10" s="24" t="b">
         <v>0</v>
       </c>
+      <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
@@ -2206,6 +2207,7 @@
       <c r="C11" s="24" t="b">
         <v>0</v>
       </c>
+      <c r="D11" s="28"/>
     </row>
     <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
depend on app settings
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C0248E-C428-4FA6-89A2-53CFDE39768D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A15EE1-4EC8-43ED-B90F-4039B4E902F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11235" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-19725" yWindow="1185" windowWidth="17280" windowHeight="10005" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -2092,7 +2092,7 @@
       </c>
       <c r="E1" s="25" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C993), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C993))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 10 PERCENT = 0%</v>
+        <v>UPDATE = 8 OUT OF 10 PERCENT = 80%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2104,7 +2104,7 @@
         <v>86</v>
       </c>
       <c r="C2" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="28"/>
     </row>
@@ -2125,7 +2125,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2145,7 +2145,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="28"/>
     </row>
@@ -2157,7 +2157,7 @@
         <v>89</v>
       </c>
       <c r="C7" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="28"/>
     </row>
@@ -2169,7 +2169,7 @@
         <v>90</v>
       </c>
       <c r="C8" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="28"/>
     </row>
@@ -2181,7 +2181,7 @@
         <v>91</v>
       </c>
       <c r="C9" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="28"/>
     </row>
@@ -2193,7 +2193,7 @@
         <v>83</v>
       </c>
       <c r="C10" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="28"/>
     </row>
@@ -2205,7 +2205,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="24" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="28"/>
     </row>

</xml_diff>

<commit_message>
AUTOMATE-15: Added test result validation
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45A15EE1-4EC8-43ED-B90F-4039B4E902F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19725" yWindow="1185" windowWidth="17280" windowHeight="10005" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1113,6 +1113,9 @@
   </si>
   <si>
     <t>Edit Guardian</t>
+  </si>
+  <si>
+    <t>View Guardian</t>
   </si>
 </sst>
 </file>
@@ -2062,10 +2065,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F26"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2091,8 +2094,8 @@
         <v>88</v>
       </c>
       <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C993), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C993))*100,2), "%")</f>
-        <v>UPDATE = 8 OUT OF 10 PERCENT = 80%</v>
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2104,7 +2107,7 @@
         <v>86</v>
       </c>
       <c r="C2" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="28"/>
     </row>
@@ -2118,98 +2121,107 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="1"/>
+      <c r="B4" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="D4" s="28"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="29" t="s">
         <v>1</v>
-      </c>
-      <c r="C4" s="24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="29" t="s">
-        <v>2</v>
       </c>
       <c r="C5" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C6" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" s="28"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="C7" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C8" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D8" s="28"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C9" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D9" s="28"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C10" s="24" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" s="28"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C11" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B12" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="24" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C12" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D12" s="28"/>
+    </row>
     <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2218,14 +2230,15 @@
     <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C11">
+  <conditionalFormatting sqref="C2:C12">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
API-4269: Added test result
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BA85E8-C548-4C23-975D-81C338586065}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>View Guardian</t>
+  </si>
+  <si>
+    <t>Print Guardian</t>
   </si>
 </sst>
 </file>
@@ -2065,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,8 +2097,8 @@
         <v>88</v>
       </c>
       <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C995), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C995))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 12 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2131,43 +2134,41 @@
       <c r="D4" s="28"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="29" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C5" s="24" t="b">
         <v>0</v>
       </c>
+      <c r="D5" s="28"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" s="29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="24" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>78</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="C8" s="24" t="b">
         <v>0</v>
@@ -2176,10 +2177,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="24" t="b">
         <v>0</v>
@@ -2188,10 +2189,10 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="24" t="b">
         <v>0</v>
@@ -2200,10 +2201,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" s="24" t="b">
         <v>0</v>
@@ -2212,17 +2213,28 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2231,14 +2243,15 @@
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
API-4271: Add edit EBM Only Order
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E6459D-3EF5-4189-AB45-B7E33D5EC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="22932" yWindow="-2424" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="95">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1116,6 +1116,9 @@
   </si>
   <si>
     <t>View Guardian</t>
+  </si>
+  <si>
+    <t>Edit EBM Only Order</t>
   </si>
 </sst>
 </file>
@@ -2065,10 +2068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2094,8 +2097,8 @@
         <v>88</v>
       </c>
       <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C995), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C995))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 12 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2163,11 +2166,9 @@
       <c r="D7" s="28"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="C8" s="24" t="b">
         <v>0</v>
@@ -2176,10 +2177,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="24" t="b">
         <v>0</v>
@@ -2188,10 +2189,10 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="24" t="b">
         <v>0</v>
@@ -2200,10 +2201,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" s="24" t="b">
         <v>0</v>
@@ -2212,17 +2213,28 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
     <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2231,14 +2243,15 @@
     <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
API-4352: Edit DBM Only & EBM or DBM Order
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E6459D-3EF5-4189-AB45-B7E33D5EC3AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{535A6458-136F-43B5-951D-6E0161C9D148}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-2424" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -205,9 +205,6 @@
     <t>Edit Patient</t>
   </si>
   <si>
-    <t>Add Order</t>
-  </si>
-  <si>
     <t>Manage Guardian</t>
   </si>
   <si>
@@ -1118,7 +1115,10 @@
     <t>View Guardian</t>
   </si>
   <si>
-    <t>Edit EBM Only Order</t>
+    <t>Edit Breastmik order</t>
+  </si>
+  <si>
+    <t>Add Breastmik Order</t>
   </si>
 </sst>
 </file>
@@ -2071,7 +2071,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2085,16 +2085,16 @@
   <sheetData>
     <row r="1" spans="1:6" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>77</v>
-      </c>
       <c r="D1" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E1" s="25" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C995), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C995))*100,2), "%")</f>
@@ -2104,10 +2104,10 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C2" s="24" t="b">
         <v>0</v>
@@ -2117,7 +2117,7 @@
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" s="24" t="b">
         <v>0</v>
@@ -2126,7 +2126,7 @@
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
       <c r="B4" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C4" s="24" t="b">
         <v>0</v>
@@ -2155,10 +2155,10 @@
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="C7" s="24" t="b">
         <v>0</v>
@@ -2168,7 +2168,7 @@
     <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C8" s="24" t="b">
         <v>0</v>
@@ -2177,10 +2177,10 @@
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C9" s="24" t="b">
         <v>0</v>
@@ -2189,10 +2189,10 @@
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C10" s="24" t="b">
         <v>0</v>
@@ -2201,10 +2201,10 @@
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C11" s="24" t="b">
         <v>0</v>
@@ -2213,10 +2213,10 @@
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="29" t="s">
         <v>82</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>83</v>
       </c>
       <c r="C12" s="24" t="b">
         <v>0</v>
@@ -2225,10 +2225,10 @@
     </row>
     <row r="13" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="29" t="s">
         <v>84</v>
-      </c>
-      <c r="B13" s="29" t="s">
-        <v>85</v>
       </c>
       <c r="C13" s="24" t="b">
         <v>0</v>
@@ -2280,45 +2280,45 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D5" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2326,13 +2326,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -2340,46 +2340,46 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D10" t="e" vm="3">
         <v>#VALUE!</v>
@@ -2387,13 +2387,13 @@
     </row>
     <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D11" t="e" vm="4">
         <v>#VALUE!</v>
@@ -2401,13 +2401,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D12" t="e" vm="5">
         <v>#VALUE!</v>
@@ -2422,38 +2422,38 @@
     </row>
     <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="37" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="D17" t="e" vm="6">
         <v>#VALUE!</v>
@@ -2461,13 +2461,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D18" t="e" vm="7">
         <v>#VALUE!</v>
@@ -2475,13 +2475,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="D19" t="e" vm="8">
         <v>#VALUE!</v>
@@ -2489,13 +2489,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D20" t="e" vm="9">
         <v>#VALUE!</v>
@@ -2503,24 +2503,24 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D22" t="e" vm="3">
         <v>#VALUE!</v>
@@ -2528,13 +2528,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D23" t="e" vm="4">
         <v>#VALUE!</v>
@@ -2542,24 +2542,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D25" t="e" vm="10">
         <v>#VALUE!</v>
@@ -2567,13 +2567,13 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D26" t="e" vm="11">
         <v>#VALUE!</v>
@@ -2581,67 +2581,67 @@
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
     </row>
     <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="C30" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="D33" t="e" vm="12">
         <v>#VALUE!</v>
@@ -2649,13 +2649,13 @@
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="D34" t="e" vm="13">
         <v>#VALUE!</v>
@@ -2663,13 +2663,13 @@
     </row>
     <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="D35" t="e" vm="14">
         <v>#VALUE!</v>
@@ -2677,24 +2677,24 @@
     </row>
     <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2791,7 +2791,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update test result alignment
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C3E6895-9189-4A03-8899-56968C2251D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386EFE5-678E-4813-AA45-1CF76400B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -1618,6 +1618,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1642,18 +1648,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2149,8 +2149,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2188,7 +2188,7 @@
       <c r="B2" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="38" t="b">
+      <c r="C2" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D2" s="27"/>
@@ -2198,7 +2198,7 @@
       <c r="B3" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C3" s="38" t="b">
+      <c r="C3" s="40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2206,7 +2206,7 @@
       <c r="B4" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="38" t="b">
+      <c r="C4" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="27"/>
@@ -2216,7 +2216,7 @@
       <c r="B5" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="C5" s="38" t="b">
+      <c r="C5" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="27"/>
@@ -2228,7 +2228,7 @@
       <c r="B6" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="b">
+      <c r="C6" s="40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2237,52 +2237,52 @@
       <c r="B7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="38" t="b">
+      <c r="C7" s="40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="C8" s="38" t="b">
+      <c r="C8" s="40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="30" t="s">
         <v>95</v>
       </c>
-      <c r="C9" s="38" t="b">
+      <c r="C9" s="40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="38" t="b">
+      <c r="C10" s="40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="C11" s="38" t="b">
+      <c r="C11" s="40" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="30" t="s">
         <v>98</v>
       </c>
-      <c r="C12" s="38" t="b">
+      <c r="C12" s="40" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2290,40 +2290,40 @@
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="29" t="s">
         <v>101</v>
       </c>
-      <c r="C13" s="38" t="b">
+      <c r="C13" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D13" s="27"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C14" s="38" t="b">
+      <c r="C14" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="27"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="38" t="b">
+      <c r="C15" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="27"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="38" t="b">
+      <c r="C16" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D16" s="27"/>
@@ -2335,7 +2335,7 @@
       <c r="B17" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C17" s="38" t="b">
+      <c r="C17" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="27"/>
@@ -2347,67 +2347,67 @@
       <c r="B18" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C18" s="38" t="b">
+      <c r="C18" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="27"/>
     </row>
     <row r="19" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="39" t="s">
+      <c r="B19" s="29" t="s">
         <v>103</v>
       </c>
-      <c r="C19" s="38" t="b">
+      <c r="C19" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D19" s="27"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C20" s="38" t="b">
+      <c r="C20" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D20" s="27"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C21" s="38" t="b">
+      <c r="C21" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="27"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C22" s="38" t="b">
+      <c r="C22" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="27"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="C23" s="38" t="b">
+      <c r="C23" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="27"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="40" t="s">
+      <c r="B24" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="C24" s="38" t="b">
+      <c r="C24" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="27"/>
@@ -2419,7 +2419,7 @@
       <c r="B25" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="38" t="b">
+      <c r="C25" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D25" s="27"/>
@@ -2431,7 +2431,7 @@
       <c r="B26" s="28" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="38" t="b">
+      <c r="C26" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D26" s="27"/>
@@ -2443,7 +2443,7 @@
       <c r="B27" s="28" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="38" t="b">
+      <c r="C27" s="40" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="27"/>
@@ -2493,25 +2493,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="35"/>
-      <c r="C1" s="35"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -2628,25 +2628,25 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="34" t="s">
+      <c r="A13" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="36" t="s">
+      <c r="A14" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="37"/>
-      <c r="C14" s="37"/>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -2794,11 +2794,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="31"/>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
     </row>
     <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
@@ -2808,11 +2808,11 @@
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="32" t="s">
+      <c r="A29" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="33"/>
-      <c r="C29" s="33"/>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">

</xml_diff>

<commit_message>
Update remarks column width
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386EFE5-678E-4813-AA45-1CF76400B01A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170F633-79E8-4D82-A467-87083F5F7164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -19,7 +19,6 @@
     <sheet name="Patient" sheetId="6" r:id="rId4"/>
     <sheet name="Patient Feeding Order" sheetId="7" r:id="rId5"/>
     <sheet name="Print &amp; Receive CollectionLabel" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1069,11 +1068,6 @@
   </si>
   <si>
     <t>Add Guardian</t>
-  </si>
-  <si>
-    <t>•Add Guardian
-     •Expected output: 
-     •Actual Output:</t>
   </si>
   <si>
     <r>
@@ -1531,7 +1525,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1606,9 +1600,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1623,29 +1614,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1654,6 +1622,29 @@
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2150,7 +2141,7 @@
   <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C27"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,7 +2149,7 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="4" max="4" width="113" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2172,8 +2163,8 @@
       <c r="C1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>87</v>
+      <c r="D1" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="E1" s="24" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1009), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1009))*100,2), "%")</f>
@@ -2185,104 +2176,104 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>85</v>
       </c>
-      <c r="C2" s="40" t="b">
+      <c r="C2" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="27"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="40" t="b">
+      <c r="B3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="40" t="b">
+      <c r="B4" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="27"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="C5" s="40" t="b">
+      <c r="B5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D5" s="27"/>
+      <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="40" t="b">
+      <c r="C6" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="40" t="b">
+      <c r="C7" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
-      <c r="B8" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="C8" s="40" t="b">
+      <c r="B8" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="B9" s="30" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="40" t="b">
+      <c r="B9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="C10" s="40" t="b">
+      <c r="B10" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="B11" s="30" t="s">
-        <v>97</v>
-      </c>
-      <c r="C11" s="40" t="b">
+      <c r="B11" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="30" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="30" t="s">
-        <v>98</v>
-      </c>
-      <c r="C12" s="40" t="b">
+      <c r="B12" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="30" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2290,163 +2281,163 @@
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>101</v>
-      </c>
-      <c r="C13" s="40" t="b">
+      <c r="B13" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D13" s="27"/>
+      <c r="D13" s="26"/>
     </row>
     <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="B14" s="30" t="s">
-        <v>102</v>
-      </c>
-      <c r="C14" s="40" t="b">
+      <c r="B14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D14" s="27"/>
+      <c r="D14" s="26"/>
     </row>
     <row r="15" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="B15" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="C15" s="40" t="b">
+      <c r="B15" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D15" s="27"/>
+      <c r="D15" s="26"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="B16" s="30" t="s">
-        <v>100</v>
-      </c>
-      <c r="C16" s="40" t="b">
+      <c r="B16" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D16" s="27"/>
+      <c r="D16" s="26"/>
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="40" t="b">
+      <c r="B17" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D17" s="27"/>
+      <c r="D17" s="26"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="40" t="b">
+      <c r="B18" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D18" s="27"/>
+      <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="B19" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="40" t="b">
+      <c r="B19" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D19" s="27"/>
+      <c r="D19" s="26"/>
     </row>
     <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="B20" s="30" t="s">
-        <v>104</v>
-      </c>
-      <c r="C20" s="40" t="b">
+      <c r="B20" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D20" s="27"/>
+      <c r="D20" s="26"/>
     </row>
     <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="B21" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="40" t="b">
+      <c r="B21" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D21" s="27"/>
+      <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
-      <c r="B22" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="C22" s="40" t="b">
+      <c r="B22" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="27"/>
+      <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
-      <c r="B23" s="30" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="40" t="b">
+      <c r="B23" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D23" s="27"/>
+      <c r="D23" s="26"/>
     </row>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="30" t="s">
-        <v>108</v>
-      </c>
-      <c r="C24" s="40" t="b">
+      <c r="B24" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D24" s="27"/>
+      <c r="D24" s="26"/>
     </row>
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="28" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="40" t="b">
+      <c r="B25" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D25" s="27"/>
+      <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="28" t="s">
+      <c r="B26" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="40" t="b">
+      <c r="C26" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D26" s="27"/>
+      <c r="D26" s="26"/>
     </row>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="27" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="40" t="b">
+      <c r="C27" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D27" s="27"/>
+      <c r="D27" s="26"/>
     </row>
     <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2990,25 +2981,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600FDF5B-AFBA-4D0E-8291-7FBB5CFF59D0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
-        <v>86</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
API-4370: Create scenario steps
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170F633-79E8-4D82-A467-87083F5F7164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,6 @@
     <sheet name="Patient" sheetId="6" r:id="rId4"/>
     <sheet name="Patient Feeding Order" sheetId="7" r:id="rId5"/>
     <sheet name="Print &amp; Receive CollectionLabel" sheetId="8" r:id="rId6"/>
-    <sheet name="Sheet1" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -203,9 +202,6 @@
   </si>
   <si>
     <t>Edit Patient</t>
-  </si>
-  <si>
-    <t>Add Order</t>
   </si>
   <si>
     <t>Manage Guardian</t>
@@ -1074,11 +1070,6 @@
     <t>Add Guardian</t>
   </si>
   <si>
-    <t>•Add Guardian
-     •Expected output: 
-     •Actual Output:</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -1116,6 +1107,54 @@
   </si>
   <si>
     <t>View Guardian</t>
+  </si>
+  <si>
+    <t>Print Guardian</t>
+  </si>
+  <si>
+    <t>Print Patient</t>
+  </si>
+  <si>
+    <t>View Patient</t>
+  </si>
+  <si>
+    <t>Discharge Patient</t>
+  </si>
+  <si>
+    <t>View Mother Info</t>
+  </si>
+  <si>
+    <t>Feeding Report</t>
+  </si>
+  <si>
+    <t>View Order</t>
+  </si>
+  <si>
+    <t>Order List</t>
+  </si>
+  <si>
+    <t>Add Order</t>
+  </si>
+  <si>
+    <t>Edit Order</t>
+  </si>
+  <si>
+    <t>Receive Donor Bottles (MBMS)</t>
+  </si>
+  <si>
+    <t>Receive Donor Bottles</t>
+  </si>
+  <si>
+    <t>Receive Product RTU/ RTF</t>
+  </si>
+  <si>
+    <t>Receive Product FPR</t>
+  </si>
+  <si>
+    <t>Receive Product Medolac</t>
+  </si>
+  <si>
+    <t>Receive Product Prolacta</t>
   </si>
 </sst>
 </file>
@@ -1295,7 +1334,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1451,12 +1490,42 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thick">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1528,27 +1597,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
           <xfpb:xfComplement i="0"/>
         </ext>
       </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2065,10 +2138,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2076,169 +2149,313 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
+    <col min="4" max="4" width="113" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="C1" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="25" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
+      <c r="D1" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E1" s="24" t="str">
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1009), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1009))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 26 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="29" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" s="24" t="b">
+        <v>3</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="C2" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D2" s="28"/>
+      <c r="D2" s="26"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="C3" s="24" t="b">
+      <c r="C4" s="30" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="B4" s="29" t="s">
+      <c r="D4" s="26"/>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" s="26"/>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="24" t="b">
+      <c r="C8" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
+    </row>
+    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="B5" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="24" t="b">
+    </row>
+    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="24" t="b">
+    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="C12" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C13" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="26"/>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D14" s="26"/>
+    </row>
+    <row r="15" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="28" t="s">
+        <v>98</v>
+      </c>
+      <c r="C15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="24" t="b">
+      <c r="B17" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B18" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="19" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="28" t="s">
+        <v>102</v>
+      </c>
+      <c r="C19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D22" s="26"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D23" s="26"/>
+    </row>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D24" s="26"/>
+    </row>
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C8" s="24" t="b">
+      <c r="C25" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D8" s="28"/>
-    </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="29" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="24" t="b">
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="C26" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="24" t="b">
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D10" s="28"/>
-    </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="D11" s="28"/>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="B12" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="24" t="b">
-        <v>0</v>
-      </c>
-      <c r="D12" s="28"/>
-    </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
+  <conditionalFormatting sqref="C2:C27">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -2247,6 +2464,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2266,46 +2484,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+    </row>
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-    </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="37" t="s">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+    </row>
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-    </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="31"/>
-      <c r="C3" s="31"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D5" t="e" vm="1">
         <v>#VALUE!</v>
@@ -2313,13 +2531,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>14</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>15</v>
       </c>
       <c r="D6" t="e" vm="2">
         <v>#VALUE!</v>
@@ -2327,46 +2545,46 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="C7" s="5" t="s">
         <v>17</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="C8" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="D10" t="e" vm="3">
         <v>#VALUE!</v>
@@ -2374,13 +2592,13 @@
     </row>
     <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="D11" t="e" vm="4">
         <v>#VALUE!</v>
@@ -2388,59 +2606,59 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>32</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>33</v>
       </c>
       <c r="D12" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35" t="s">
+      <c r="A13" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="37"/>
     </row>
     <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="37" t="s">
+      <c r="A14" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39"/>
+    </row>
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-    </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="31"/>
-      <c r="C15" s="31"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="32"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="C16" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="D17" t="e" vm="6">
         <v>#VALUE!</v>
@@ -2448,13 +2666,13 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>38</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>39</v>
       </c>
       <c r="D18" t="e" vm="7">
         <v>#VALUE!</v>
@@ -2462,13 +2680,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>40</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>41</v>
       </c>
       <c r="D19" t="e" vm="8">
         <v>#VALUE!</v>
@@ -2476,13 +2694,13 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D20" t="e" vm="9">
         <v>#VALUE!</v>
@@ -2490,24 +2708,24 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="D22" t="e" vm="3">
         <v>#VALUE!</v>
@@ -2515,13 +2733,13 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B23" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="D23" t="e" vm="4">
         <v>#VALUE!</v>
@@ -2529,24 +2747,24 @@
     </row>
     <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>54</v>
       </c>
       <c r="D25" t="e" vm="10">
         <v>#VALUE!</v>
@@ -2554,81 +2772,81 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D26" t="e" vm="11">
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="32" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="32"/>
+      <c r="A27" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="33"/>
+      <c r="C27" s="33"/>
     </row>
     <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="B29" s="34"/>
-      <c r="C29" s="34"/>
+      <c r="A29" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="35"/>
+      <c r="C29" s="35"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="C30" s="9" t="s">
         <v>8</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="12" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="15" t="s">
         <v>65</v>
-      </c>
-      <c r="C33" s="15" t="s">
-        <v>66</v>
       </c>
       <c r="D33" t="e" vm="12">
         <v>#VALUE!</v>
@@ -2636,13 +2854,13 @@
     </row>
     <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B34" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>67</v>
-      </c>
-      <c r="C34" s="17" t="s">
-        <v>68</v>
       </c>
       <c r="D34" t="e" vm="13">
         <v>#VALUE!</v>
@@ -2650,13 +2868,13 @@
     </row>
     <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B35" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="C35" s="19" t="s">
         <v>69</v>
-      </c>
-      <c r="C35" s="19" t="s">
-        <v>70</v>
       </c>
       <c r="D35" t="e" vm="14">
         <v>#VALUE!</v>
@@ -2664,24 +2882,24 @@
     </row>
     <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C36" s="19" t="s">
         <v>71</v>
-      </c>
-      <c r="C36" s="19" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>73</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -2763,25 +2981,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{600FDF5B-AFBA-4D0E-8291-7FBB5CFF59D0}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" ht="135" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
API-4268 Automation - Manage Guardian | UI Verification
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\client-notes\automation\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2DF30E2-13EE-4A3A-861B-6ED3355560D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="33810" yWindow="3930" windowWidth="17280" windowHeight="9960" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1116,6 +1116,22 @@
   </si>
   <si>
     <t>View Guardian</t>
+  </si>
+  <si>
+    <t>Manage Guardian UI Verification</t>
+  </si>
+  <si>
+    <t>• Guardian UI Verification 
+     • Expected output:
+      mother/track/visit_number = False
+      ui/text/visit_number = Visit Number
+      ui/text/mrn_number = MRN
+      ui/text/account_number = FIN
+     • Actual Output:
+      mother/track/visit_number = False
+      ui/text/visit_number = 
+      ui/text/mrn_number = MRN:
+      ui/text/account_number = FIN:</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1139,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1521,7 +1537,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2065,22 +2081,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>75</v>
       </c>
@@ -2094,12 +2110,12 @@
         <v>88</v>
       </c>
       <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C995), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C995))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 12 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2111,7 +2127,7 @@
       </c>
       <c r="D2" s="28"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="29" t="s">
         <v>92</v>
@@ -2120,7 +2136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="29" t="s">
         <v>93</v>
@@ -2130,115 +2146,127 @@
       </c>
       <c r="D4" s="28"/>
     </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
+    <row r="5" spans="1:6" ht="159" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
       <c r="B5" s="29" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C5" s="24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="D5" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" s="29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>78</v>
-      </c>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
       <c r="B7" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="C8" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="28"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="28"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="28"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -2258,35 +2286,35 @@
       <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2297,7 +2325,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2339,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2325,7 +2353,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2336,7 +2364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -2347,7 +2375,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2358,7 +2386,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2372,7 +2400,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -2386,7 +2414,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -2400,28 +2428,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2432,7 +2460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -2446,7 +2474,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -2460,7 +2488,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2474,7 +2502,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2488,7 +2516,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2499,7 +2527,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -2513,7 +2541,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -2527,7 +2555,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -2538,7 +2566,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2552,7 +2580,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
@@ -2566,28 +2594,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
     </row>
-    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>7</v>
       </c>
@@ -2598,7 +2626,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2637,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>13</v>
       </c>
@@ -2620,7 +2648,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>16</v>
       </c>
@@ -2634,7 +2662,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>19</v>
       </c>
@@ -2648,7 +2676,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>22</v>
       </c>
@@ -2662,7 +2690,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +2701,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>28</v>
       </c>
@@ -2684,20 +2712,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="23"/>
       <c r="C39" s="21"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="23"/>
     </row>
@@ -2723,7 +2751,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2735,7 +2763,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2747,7 +2775,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2759,7 +2787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2771,12 +2799,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
API-4370: With updated test result
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170F633-79E8-4D82-A467-87083F5F7164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9D194D-9A72-4D63-B6DF-7761BA625F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -2140,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,7 +2149,7 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="113" customWidth="1"/>
+    <col min="4" max="4" width="141.7109375" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2240,6 +2240,7 @@
       <c r="C8" s="30" t="b">
         <v>0</v>
       </c>
+      <c r="D8" s="26"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>

</xml_diff>

<commit_message>
API-4371: Complete discharge patient test case
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC9D194D-9A72-4D63-B6DF-7761BA625F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D141872A-B2B0-47FD-9FB3-789CB127D273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-1500" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -2140,8 +2140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,7 +2168,7 @@
       </c>
       <c r="E1" s="24" t="str">
         <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1009), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1009))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 26 PERCENT = 0%</v>
+        <v>UPDATE = 1 OUT OF 26 PERCENT = 3.85%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
@@ -2257,8 +2257,9 @@
         <v>95</v>
       </c>
       <c r="C10" s="30" t="b">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D10" s="26"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>

</xml_diff>

<commit_message>
Added update base on peer review comment like fixing the InTestResult condition
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\uipath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D91DC-F2E6-44E2-93B0-06A6777CF6B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6DC43-7FAD-4A82-AAC2-13A1DED7C887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1860" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView minimized="1" xWindow="32940" yWindow="3060" windowWidth="17280" windowHeight="9960" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="96">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1116,6 +1116,29 @@
   </si>
   <si>
     <t>View Guardian</t>
+  </si>
+  <si>
+    <t>Manage Guardian UI Verification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Guardian UI Verification 
+    • Expected output:
+        Guardian List Header = 2
+        MRN Settings Text = MRN
+        Account Number Text = FIN
+        First Name Validation Msg = First Name is required.
+        Last Name Validation Msg = Last Name is required.
+        MRN Validation Msg = MRN is required.
+        FIN Validation Msg = FIN is required
+    • Actual Output:
+        Guardian List Header = Account Number
+        MRN Settings Text = MRN:
+        Account Number Text = FIN:
+        First Name Validation Msg = First Name is required.
+        Last Name Validation Msg = Last Name is required.
+        MRN Validation Msg = MRN is required.
+        FIN Validation Msg = FIN is required
+</t>
   </si>
 </sst>
 </file>
@@ -1123,7 +1146,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1521,7 +1544,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -2065,22 +2088,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="67.5703125" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="4" max="4" width="67.5546875" customWidth="1"/>
+    <col min="5" max="5" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
         <v>75</v>
       </c>
@@ -2094,12 +2117,12 @@
         <v>88</v>
       </c>
       <c r="E1" s="25" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C994), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C994))*100,2), "%")</f>
-        <v>UPDATE = 0 OUT OF 11 PERCENT = 0%</v>
+        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C995), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C995))*100,2), "%")</f>
+        <v>UPDATE = 0 OUT OF 12 PERCENT = 0%</v>
       </c>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -2111,7 +2134,7 @@
       </c>
       <c r="D2" s="28"/>
     </row>
-    <row r="3" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="29" t="s">
         <v>92</v>
@@ -2120,7 +2143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="29" t="s">
         <v>93</v>
@@ -2128,117 +2151,128 @@
       <c r="C4" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="D4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
+    </row>
+    <row r="5" spans="1:6" ht="274.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="1"/>
       <c r="B5" s="29" t="s">
-        <v>1</v>
+        <v>94</v>
       </c>
       <c r="C5" s="24" t="b">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
+      <c r="D5" s="28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B6" s="29" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C6" s="24" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>78</v>
-      </c>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1"/>
       <c r="B7" s="29" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C7" s="24" t="b">
         <v>0</v>
       </c>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="29" t="s">
-        <v>89</v>
+        <v>3</v>
       </c>
       <c r="C8" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D8" s="28"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C9" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D9" s="28"/>
     </row>
-    <row r="10" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C10" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D10" s="28"/>
     </row>
-    <row r="11" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="C11" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D11" s="28"/>
     </row>
-    <row r="12" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B12" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C12" s="24" t="b">
         <v>0</v>
       </c>
       <c r="D12" s="28"/>
     </row>
-    <row r="13" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B13" s="29" t="s">
+        <v>85</v>
+      </c>
+      <c r="C13" s="24" t="b">
+        <v>0</v>
+      </c>
+      <c r="D13" s="28"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="15" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="17" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="18" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="19" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="20" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="21" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="22" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="23" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="24" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="26" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="27" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="28" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C12">
+  <conditionalFormatting sqref="C2:C13">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -2258,35 +2292,35 @@
       <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="35" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="36"/>
       <c r="C1" s="36"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="38"/>
       <c r="C2" s="38"/>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="30" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="31"/>
       <c r="C3" s="31"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -2297,7 +2331,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -2311,7 +2345,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
@@ -2325,7 +2359,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>16</v>
       </c>
@@ -2336,7 +2370,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>19</v>
       </c>
@@ -2347,7 +2381,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2358,7 +2392,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>25</v>
       </c>
@@ -2372,7 +2406,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>28</v>
       </c>
@@ -2386,7 +2420,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>31</v>
       </c>
@@ -2400,28 +2434,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="35" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="36"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="37" t="s">
         <v>34</v>
       </c>
       <c r="B14" s="38"/>
       <c r="C14" s="38"/>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="30" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="31"/>
       <c r="C15" s="31"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -2432,7 +2466,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>10</v>
       </c>
@@ -2446,7 +2480,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>13</v>
       </c>
@@ -2460,7 +2494,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -2474,7 +2508,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -2488,7 +2522,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2499,7 +2533,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>25</v>
       </c>
@@ -2513,7 +2547,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>28</v>
       </c>
@@ -2527,7 +2561,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>31</v>
       </c>
@@ -2538,7 +2572,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>52</v>
       </c>
@@ -2552,7 +2586,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>55</v>
       </c>
@@ -2566,28 +2600,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="32" t="s">
         <v>58</v>
       </c>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
     </row>
-    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>59</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="33" t="s">
         <v>60</v>
       </c>
       <c r="B29" s="34"/>
       <c r="C29" s="34"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>7</v>
       </c>
@@ -2598,7 +2632,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>10</v>
       </c>
@@ -2609,7 +2643,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>13</v>
       </c>
@@ -2620,7 +2654,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>16</v>
       </c>
@@ -2634,7 +2668,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>19</v>
       </c>
@@ -2648,7 +2682,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>22</v>
       </c>
@@ -2662,7 +2696,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>25</v>
       </c>
@@ -2673,7 +2707,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>28</v>
       </c>
@@ -2684,20 +2718,20 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="23"/>
       <c r="C39" s="21"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="23"/>
     </row>
@@ -2723,7 +2757,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2735,7 +2769,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2747,7 +2781,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2759,7 +2793,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2771,12 +2805,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="135" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>87</v>
       </c>

</xml_diff>

<commit_message>
Updates from previous demo
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -2,24 +2,23 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Documents\UiPath\TMNP Smoke Testing Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{487A5AF3-EF8E-4F26-9F0C-F82B92606310}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C97E8A5-9996-43B5-8BDB-46BE11C2C6D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1560" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart1" sheetId="9" r:id="rId1"/>
-    <sheet name="Test Result" sheetId="1" r:id="rId2"/>
-    <sheet name="Sample" sheetId="2" r:id="rId3"/>
-    <sheet name="Guardian" sheetId="5" r:id="rId4"/>
-    <sheet name="Patient" sheetId="6" r:id="rId5"/>
-    <sheet name="Patient Feeding Order" sheetId="7" r:id="rId6"/>
-    <sheet name="Print &amp; Receive CollectionLabel" sheetId="8" r:id="rId7"/>
+    <sheet name="Test Result" sheetId="1" r:id="rId1"/>
+    <sheet name="Sample" sheetId="2" r:id="rId2"/>
+    <sheet name="Guardian" sheetId="5" r:id="rId3"/>
+    <sheet name="Patient" sheetId="6" r:id="rId4"/>
+    <sheet name="Patient Feeding Order" sheetId="7" r:id="rId5"/>
+    <sheet name="Print &amp; Receive CollectionLabel" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -194,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="121">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1065,9 +1064,6 @@
     <t>Feed</t>
   </si>
   <si>
-    <t>Dosed EHM</t>
-  </si>
-  <si>
     <t>Add Guardian</t>
   </si>
   <si>
@@ -1101,9 +1097,6 @@
     <t>Guardian Container</t>
   </si>
   <si>
-    <t>EHM Only</t>
-  </si>
-  <si>
     <t>Edit Guardian</t>
   </si>
   <si>
@@ -1156,6 +1149,51 @@
   </si>
   <si>
     <t>Receive Product Prolacta</t>
+  </si>
+  <si>
+    <t>Scan fortified container multiple times</t>
+  </si>
+  <si>
+    <t>EHM + Fortifier</t>
+  </si>
+  <si>
+    <t>Prepared EHM + Fortifier</t>
+  </si>
+  <si>
+    <t>EHM + Fortifier + Modular</t>
+  </si>
+  <si>
+    <t>Prepared EHM + Fortifier + Modular</t>
+  </si>
+  <si>
+    <t>RTU without fortifier</t>
+  </si>
+  <si>
+    <t>Prepared RTU without fortifier</t>
+  </si>
+  <si>
+    <t>Water + Powder + Fortifier</t>
+  </si>
+  <si>
+    <t>Prepared Water + Powder + Fortifier</t>
+  </si>
+  <si>
+    <t>Fresh EHM Container</t>
+  </si>
+  <si>
+    <t>Prepared Fresh EHM Container</t>
+  </si>
+  <si>
+    <t>Thawed EHM Container</t>
+  </si>
+  <si>
+    <t>Prepared Thawed EHM Container</t>
+  </si>
+  <si>
+    <t>Fresh &amp; Thawed EHM Container</t>
+  </si>
+  <si>
+    <t>Prepared Fresh &amp; Thawed EHM Container</t>
   </si>
 </sst>
 </file>
@@ -1335,7 +1373,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1521,12 +1559,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thick">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1624,6 +1682,15 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1691,304 +1758,25 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Test Result'!$H$1:$I$1</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>Total: 26</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Pass: 7</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Test Result'!$H$2:$I$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>26</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E4A7-407A-ABEF-C06068E34240}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="1552793487"/>
-        <c:axId val="1552790607"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1552793487"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1552790607"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="1552790607"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1552793487"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
       <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Test</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Result</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
+        <c:strRef>
+          <c:f>'Test Result'!$T$1</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>0 OUT OF 39 
+PERCENT = 0%</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
       </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -2037,6 +1825,11 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-1BE8-4171-A39B-CB41D7E2EA38}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dPt>
             <c:idx val="1"/>
@@ -2052,35 +1845,40 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-1BE8-4171-A39B-CB41D7E2EA38}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
             <c:delete val="1"/>
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Test Result'!$H$1:$I$1</c:f>
+              <c:f>'Test Result'!$V$1:$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Total: 26</c:v>
+                  <c:v>Failed or not yet done: 39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Pass: 7</c:v>
+                  <c:v>Passed: 0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Test Result'!$H$2:$I$2</c:f>
+              <c:f>'Test Result'!$V$2:$W$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>26</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2115,7 +1913,11 @@
       <c:legendPos val="b"/>
       <c:overlay val="0"/>
       <c:spPr>
-        <a:noFill/>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -2125,8 +1927,8 @@
         <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
         <a:lstStyle/>
         <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+          <a:pPr rtl="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -2219,550 +2021,7 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3281,64 +2540,20 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{832CE900-B13C-4FD3-BFDC-3D179798E7D8}">
-  <sheetPr/>
-  <sheetViews>
-    <sheetView zoomScale="90" workbookViewId="0" zoomToFit="1"/>
-  </sheetViews>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</chartsheet>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:absoluteAnchor>
-    <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="10826750" cy="7863417"/>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5890DE8-8FD2-BA0C-46BB-2BEB0289520A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks noGrp="1"/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:absoluteAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>6250305</xdr:colOff>
+      <xdr:colOff>7408333</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>31749</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>251459</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>277070</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3515,7 +2730,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Custom 5">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3529,10 +2744,10 @@
         <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="FF0000"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="196B24"/>
       </a:accent2>
       <a:accent3>
         <a:srgbClr val="196B24"/>
@@ -3829,10 +3044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:W53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3841,10 +3056,11 @@
     <col min="2" max="2" width="25.5546875" customWidth="1"/>
     <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="113" customWidth="1"/>
-    <col min="5" max="5" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>
@@ -3855,71 +3071,72 @@
         <v>76</v>
       </c>
       <c r="D1" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="E1" s="24" t="str">
-        <f>CONCATENATE("UPDATE = ", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1009), " ", "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1009))*100,2), "%")</f>
-        <v>UPDATE = 7 OUT OF 26 PERCENT = 26.92%</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1"/>
-      <c r="H1" t="str">
-        <f>_xlfn.CONCAT("Total: ", COUNTA($C2:$C1009))</f>
-        <v>Total: 26</v>
-      </c>
-      <c r="I1" t="str">
-        <f>_xlfn.CONCAT("Pass: ", COUNTIF($C:$C,TRUE))</f>
-        <v>Pass: 7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="T1" s="24" t="str">
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1020), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1020))*100,2), "%")</f>
+        <v>0 OUT OF 39 
+PERCENT = 0%</v>
+      </c>
+      <c r="V1" t="str">
+        <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
+        <v>Failed or not yet done: 39</v>
+      </c>
+      <c r="W1" t="str">
+        <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
+        <v>Passed: 0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="26"/>
-      <c r="H2">
-        <f>COUNTA($C2:$C1009)</f>
-        <v>26</v>
-      </c>
-      <c r="I2">
-        <f>COUNTIF($C:$C,TRUE)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="V2">
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1020))*100,2)</f>
+        <v>100</v>
+      </c>
+      <c r="W2">
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1020))*100,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="C3" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="27" t="s">
-        <v>92</v>
-      </c>
       <c r="C4" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D4" s="26"/>
     </row>
-    <row r="5" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="27" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
@@ -3927,10 +3144,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="27" t="s">
         <v>2</v>
@@ -3939,87 +3156,87 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="28" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C8" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="29" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C9" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="29" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C10" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="29" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C11" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="29" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C12" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>77</v>
       </c>
       <c r="B13" s="28" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C13" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" s="26"/>
     </row>
-    <row r="14" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C14" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D14" s="26"/>
     </row>
-    <row r="15" spans="1:9" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C15" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D15" s="26"/>
     </row>
-    <row r="16" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="29" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C16" s="30" t="b">
         <v>0</v>
@@ -4031,10 +3248,10 @@
         <v>78</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C17" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" s="26"/>
     </row>
@@ -4043,17 +3260,17 @@
         <v>79</v>
       </c>
       <c r="B18" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C18" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="28" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C19" s="30" t="b">
         <v>0</v>
@@ -4063,7 +3280,7 @@
     <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="29" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C20" s="30" t="b">
         <v>0</v>
@@ -4073,27 +3290,27 @@
     <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C21" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" s="26"/>
     </row>
     <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="29" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C22" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" s="26"/>
     </row>
     <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23" s="30" t="b">
         <v>0</v>
@@ -4103,7 +3320,7 @@
     <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="29" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="30" t="b">
         <v>0</v>
@@ -4114,8 +3331,8 @@
       <c r="A25" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B25" s="27" t="s">
-        <v>89</v>
+      <c r="B25" s="33" t="s">
+        <v>115</v>
       </c>
       <c r="C25" s="30" t="b">
         <v>0</v>
@@ -4123,46 +3340,173 @@
       <c r="D25" s="26"/>
     </row>
     <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="1"/>
+      <c r="B26" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="1"/>
+      <c r="B27" s="33" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="1"/>
+      <c r="B28" s="27" t="s">
+        <v>107</v>
+      </c>
+      <c r="C28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="1"/>
+      <c r="B29" s="31" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1"/>
+      <c r="B30" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C30" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="31" t="s">
+        <v>113</v>
+      </c>
+      <c r="C31" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="26"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B32" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1" t="s">
+      <c r="C32" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+      <c r="B33" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="27" t="s">
-        <v>84</v>
-      </c>
-      <c r="C27" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="B34" s="32" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="32" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="32" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="32" t="s">
+        <v>114</v>
+      </c>
+      <c r="C40" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C27">
+  <conditionalFormatting sqref="C2:C40">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -4192,25 +3536,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="32"/>
-      <c r="C3" s="32"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -4327,25 +3671,25 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="A13" s="39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
     </row>
     <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="38" t="s">
+      <c r="A14" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="32"/>
-      <c r="C15" s="32"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="35"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
@@ -4493,11 +3837,11 @@
       </c>
     </row>
     <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="33" t="s">
+      <c r="A27" s="36" t="s">
         <v>57</v>
       </c>
-      <c r="B27" s="33"/>
-      <c r="C27" s="33"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
     </row>
     <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
@@ -4507,11 +3851,11 @@
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="B29" s="35"/>
-      <c r="C29" s="35"/>
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">

</xml_diff>

<commit_message>
Add TC for Exclusion Date
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3116FD4-B241-4BC6-860C-1928022D4FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2D6C4FF-0BF0-45CE-986B-B7E54A2FA333}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1197,6 +1197,9 @@
   </si>
   <si>
     <t>Manage Guardian UI Verification</t>
+  </si>
+  <si>
+    <t>Manage Exclusion Date</t>
   </si>
 </sst>
 </file>
@@ -1204,7 +1207,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1587,7 +1590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1652,7 +1655,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1717,6 +1720,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1767,7 +1773,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 40 
+              <c:v>0 OUT OF 41 
 PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
@@ -1863,7 +1869,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 40</c:v>
+                  <c:v>Failed or not yet done: 41</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Passed: 0</c:v>
@@ -2555,7 +2561,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>277070</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3047,23 +3053,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W54"/>
+  <dimension ref="A1:W55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5546875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
+    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
     <col min="4" max="4" width="113" customWidth="1"/>
-    <col min="5" max="5" width="45.44140625" customWidth="1"/>
-    <col min="22" max="22" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="22" max="22" width="21.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>
@@ -3078,20 +3084,20 @@
       </c>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1021), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1021))*100,2), "%")</f>
-        <v>0 OUT OF 40 
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1022), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1022))*100,2), "%")</f>
+        <v>0 OUT OF 41 
 PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 40</v>
+        <v>Failed or not yet done: 41</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
         <v>Passed: 0</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3103,15 +3109,15 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1021))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1022))*100,2)</f>
         <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1021))*100,2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1022))*100,2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="27" t="s">
         <v>88</v>
@@ -3120,7 +3126,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="27" t="s">
         <v>90</v>
       </c>
@@ -3129,7 +3135,7 @@
       </c>
       <c r="D4" s="26"/>
     </row>
-    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="27" t="s">
         <v>89</v>
@@ -3139,386 +3145,396 @@
       </c>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>121</v>
       </c>
-      <c r="C6" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="27" t="s">
-        <v>1</v>
-      </c>
       <c r="C7" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="28" t="s">
+      <c r="C9" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="C9" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="29" t="s">
-        <v>92</v>
-      </c>
       <c r="C10" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="30" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B15" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="29" t="s">
+      <c r="C15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="29" t="s">
+      <c r="C17" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+      <c r="C18" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D18" s="26"/>
+    </row>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B19" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="C18" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D18" s="26"/>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+      <c r="C19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B20" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:4" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="28" t="s">
+      <c r="C20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="29" t="s">
-        <v>101</v>
-      </c>
       <c r="C21" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D22" s="26"/>
     </row>
-    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D23" s="26"/>
     </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D24" s="26"/>
     </row>
-    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="26"/>
-    </row>
-    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+      <c r="C26" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B26" s="33" t="s">
+      <c r="B27" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C26" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="33" t="s">
-        <v>117</v>
-      </c>
       <c r="C27" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D27" s="26"/>
     </row>
-    <row r="28" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="C28" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="1"/>
-      <c r="B29" s="27" t="s">
+      <c r="C29" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="C29" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="1"/>
-      <c r="B30" s="31" t="s">
-        <v>109</v>
-      </c>
       <c r="C30" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C31" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D31" s="26"/>
     </row>
-    <row r="32" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C32" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C32" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+      <c r="C33" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B34" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C33" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A34" s="1"/>
-      <c r="B34" s="27" t="s">
+      <c r="C34" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C34" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="32" t="s">
+      <c r="B36" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C35" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="32" t="s">
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="32" t="s">
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-      <c r="B38" s="27" t="s">
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C38" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="1"/>
-      <c r="B39" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="C39" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D39" s="26"/>
     </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="1"/>
       <c r="B40" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C40" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="26"/>
     </row>
-    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C41" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="26"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C42" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C41">
+  <conditionalFormatting sqref="C2:C42">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>
@@ -3540,35 +3556,35 @@
       <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
-    <col min="2" max="2" width="46.33203125" customWidth="1"/>
-    <col min="3" max="3" width="59.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" customWidth="1"/>
+    <col min="3" max="3" width="59.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3579,7 +3595,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3593,7 +3609,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -3607,7 +3623,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3618,7 +3634,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3629,7 +3645,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3640,7 +3656,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -3654,7 +3670,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -3668,7 +3684,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -3682,28 +3698,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -3714,7 +3730,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -3728,7 +3744,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -3742,7 +3758,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -3756,7 +3772,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -3770,7 +3786,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -3781,7 +3797,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -3795,7 +3811,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -3809,7 +3825,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -3820,7 +3836,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>51</v>
       </c>
@@ -3834,7 +3850,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -3848,28 +3864,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
     </row>
-    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="37" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -3880,7 +3896,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="10" t="s">
         <v>9</v>
       </c>
@@ -3891,7 +3907,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="13" t="s">
         <v>12</v>
       </c>
@@ -3902,7 +3918,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="10" t="s">
         <v>15</v>
       </c>
@@ -3916,7 +3932,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="10" t="s">
         <v>18</v>
       </c>
@@ -3930,7 +3946,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="10" t="s">
         <v>21</v>
       </c>
@@ -3944,7 +3960,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
@@ -3955,7 +3971,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>27</v>
       </c>
@@ -3966,20 +3982,20 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="23"/>
       <c r="C39" s="21"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B41" s="21"/>
       <c r="C41" s="23"/>
     </row>
@@ -4005,7 +4021,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4017,7 +4033,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4029,7 +4045,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4041,7 +4057,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
TC for Manage Exclusion Date
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9C1857-6C7D-4338-ADCE-4C97BAE4B440}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE1E51-507C-483D-8067-1FFB86F99AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1200,6 +1200,9 @@
   </si>
   <si>
     <t>Receive Human Milk - UI Verification</t>
+  </si>
+  <si>
+    <t>Manage Exclusion Date</t>
   </si>
 </sst>
 </file>
@@ -1770,8 +1773,8 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>2 OUT OF 41 
-PERCENT = 4.88%</c:v>
+              <c:v>0 OUT OF 42 
+PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1866,10 +1869,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 39</c:v>
+                  <c:v>Failed or not yet done: 42</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Passed: 2</c:v>
+                  <c:v>Passed: 0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1881,10 +1884,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>95.12</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.88</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2558,7 +2561,7 @@
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>277070</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>171449</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3050,10 +3053,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W55"/>
+  <dimension ref="A1:W56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3081,17 +3084,17 @@
       </c>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1022), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1022))*100,2), "%")</f>
-        <v>2 OUT OF 41 
-PERCENT = 4.88%</v>
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1023), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2), "%")</f>
+        <v>0 OUT OF 42 
+PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 39</v>
+        <v>Failed or not yet done: 42</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
-        <v>Passed: 2</v>
+        <v>Passed: 0</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3106,12 +3109,12 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1022))*100,2)</f>
-        <v>95.12</v>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1023))*100,2)</f>
+        <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1022))*100,2)</f>
-        <v>4.88</v>
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3143,20 +3146,21 @@
       <c r="D5" s="26"/>
     </row>
     <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="A6" s="1"/>
+      <c r="B6" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D6" s="26"/>
+    </row>
+    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" t="s">
         <v>121</v>
-      </c>
-      <c r="C6" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="B7" s="27" t="s">
-        <v>1</v>
       </c>
       <c r="C7" s="30" t="b">
         <v>0</v>
@@ -3165,25 +3169,25 @@
     <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="28" t="s">
+      <c r="C9" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="C9" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="29" t="s">
-        <v>92</v>
       </c>
       <c r="C10" s="30" t="b">
         <v>0</v>
@@ -3192,7 +3196,7 @@
     <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="29" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C11" s="30" t="b">
         <v>0</v>
@@ -3201,7 +3205,7 @@
     <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C12" s="30" t="b">
         <v>0</v>
@@ -3210,92 +3214,91 @@
     <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="29" t="s">
+        <v>94</v>
+      </c>
+      <c r="C13" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C13" s="30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
+      <c r="C14" s="30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B15" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="C14" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D14" s="26"/>
-    </row>
-    <row r="15" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="B15" s="29" t="s">
+      <c r="C15" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D15" s="26"/>
+    </row>
+    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="C15" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D15" s="26"/>
-    </row>
-    <row r="16" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="B16" s="28" t="s">
+      <c r="C16" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="26"/>
+    </row>
+    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="C16" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="26"/>
-    </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="B17" s="29" t="s">
+      <c r="C17" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D17" s="26"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C17" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D17" s="26"/>
-    </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="B18" s="27" t="s">
-        <v>86</v>
-      </c>
       <c r="C18" s="30" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" s="26"/>
     </row>
     <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D19" s="26"/>
+    </row>
+    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B20" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C19" s="30" t="b">
-        <v>1</v>
-      </c>
-      <c r="D19" s="26"/>
-    </row>
-    <row r="20" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="28" t="s">
+      <c r="C20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="28" t="s">
         <v>100</v>
-      </c>
-      <c r="C20" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="29" t="s">
-        <v>101</v>
       </c>
       <c r="C21" s="30" t="b">
         <v>0</v>
@@ -3305,7 +3308,7 @@
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C22" s="30" t="b">
         <v>0</v>
@@ -3315,7 +3318,7 @@
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="30" t="b">
         <v>0</v>
@@ -3325,7 +3328,7 @@
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="30" t="b">
         <v>0</v>
@@ -3335,59 +3338,59 @@
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C25" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D25" s="26"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D25" s="26"/>
-    </row>
-    <row r="26" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-      <c r="B26" s="33" t="s">
+      <c r="C26" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C26" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="C27" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="33" t="s">
+      <c r="B28" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C27" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-      <c r="B28" s="33" t="s">
-        <v>117</v>
-      </c>
       <c r="C28" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D28" s="26"/>
     </row>
-    <row r="29" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
       <c r="B29" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C29" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="C29" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="C30" s="30" t="b">
         <v>0</v>
@@ -3396,8 +3399,8 @@
     </row>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
-      <c r="B31" s="31" t="s">
-        <v>109</v>
+      <c r="B31" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C31" s="30" t="b">
         <v>0</v>
@@ -3407,7 +3410,7 @@
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
       <c r="B32" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C32" s="30" t="b">
         <v>0</v>
@@ -3417,121 +3420,131 @@
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1" t="s">
+      <c r="C34" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B35" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C34" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-      <c r="B35" s="27" t="s">
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B36" s="32" t="s">
+      <c r="B37" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C36" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="32" t="s">
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="32" t="s">
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C38" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="27" t="s">
+      <c r="C39" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C39" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="C40" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D40" s="26"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="1"/>
       <c r="B41" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C41" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="26"/>
     </row>
-    <row r="42" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D42" s="26"/>
+    </row>
+    <row r="43" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C42" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D42" s="26"/>
-    </row>
-    <row r="43" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C43" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="26"/>
+    </row>
     <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C42">
+  <conditionalFormatting sqref="C2:C43">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Print Collection Label Hard and Soft Stop Verification
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DE1E51-507C-483D-8067-1FFB86F99AFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ADFEFA-1112-4082-BF66-A8E7F6F6D145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1203,6 +1203,9 @@
   </si>
   <si>
     <t>Manage Exclusion Date</t>
+  </si>
+  <si>
+    <t>Print Collection Label UI Verification - Hard and Soft Stop</t>
   </si>
 </sst>
 </file>
@@ -1773,7 +1776,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 42 
+              <c:v>0 OUT OF 43 
 PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
@@ -1869,7 +1872,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 42</c:v>
+                  <c:v>Failed or not yet done: 43</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Passed: 0</c:v>
@@ -2553,16 +2556,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>7408333</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>202406</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>31749</xdr:rowOff>
+      <xdr:rowOff>31750</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
       <xdr:colOff>277070</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>171449</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>690563</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3053,10 +3056,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W56"/>
+  <dimension ref="A1:W57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3064,7 +3067,7 @@
     <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" customWidth="1"/>
-    <col min="4" max="4" width="113" customWidth="1"/>
+    <col min="4" max="4" width="163" customWidth="1"/>
     <col min="5" max="5" width="45.42578125" customWidth="1"/>
     <col min="22" max="22" width="21.28515625" customWidth="1"/>
   </cols>
@@ -3084,13 +3087,13 @@
       </c>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1023), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2), "%")</f>
-        <v>0 OUT OF 42 
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1024), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1024))*100,2), "%")</f>
+        <v>0 OUT OF 43 
 PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 42</v>
+        <v>Failed or not yet done: 43</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
@@ -3109,11 +3112,11 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1023))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1024))*100,2)</f>
         <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1024))*100,2)</f>
         <v>0</v>
       </c>
     </row>
@@ -3283,32 +3286,32 @@
       </c>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="27" t="s">
+        <v>124</v>
+      </c>
+      <c r="C20" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D20" s="26"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B21" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" s="26"/>
-    </row>
-    <row r="21" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="28" t="s">
+      <c r="C21" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D21" s="26"/>
+    </row>
+    <row r="22" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="28" t="s">
         <v>100</v>
-      </c>
-      <c r="C21" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D21" s="26"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-      <c r="B22" s="29" t="s">
-        <v>101</v>
       </c>
       <c r="C22" s="30" t="b">
         <v>0</v>
@@ -3318,7 +3321,7 @@
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C23" s="30" t="b">
         <v>0</v>
@@ -3328,7 +3331,7 @@
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C24" s="30" t="b">
         <v>0</v>
@@ -3338,7 +3341,7 @@
     <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C25" s="30" t="b">
         <v>0</v>
@@ -3348,59 +3351,59 @@
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="C26" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D26" s="26"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="29" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D26" s="26"/>
-    </row>
-    <row r="27" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="B27" s="33" t="s">
+      <c r="C27" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D27" s="26"/>
+    </row>
+    <row r="28" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C27" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D27" s="26"/>
-    </row>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="C28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B28" s="33" t="s">
+      <c r="B29" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C28" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-      <c r="B29" s="33" t="s">
-        <v>117</v>
-      </c>
       <c r="C29" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D29" s="26"/>
     </row>
-    <row r="30" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
       <c r="B30" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C30" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="C30" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="C31" s="30" t="b">
         <v>0</v>
@@ -3409,8 +3412,8 @@
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="1"/>
-      <c r="B32" s="31" t="s">
-        <v>109</v>
+      <c r="B32" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C32" s="30" t="b">
         <v>0</v>
@@ -3420,7 +3423,7 @@
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C33" s="30" t="b">
         <v>0</v>
@@ -3430,121 +3433,131 @@
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C34" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C34" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1" t="s">
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B36" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-      <c r="B36" s="27" t="s">
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C36" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B38" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="32" t="s">
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C38" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="32" t="s">
+      <c r="C39" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-      <c r="B40" s="27" t="s">
+      <c r="C40" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C40" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="C41" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D41" s="26"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
       <c r="B42" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C42" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="26"/>
     </row>
-    <row r="43" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C43" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C43" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" s="26"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C44" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="26"/>
+    </row>
     <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C43">
+  <conditionalFormatting sqref="C2:C44">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Additional test case for prepare ebm
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{692E4BAB-71E3-4ED8-AC08-391FFCFFF7CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82376FF5-D212-425D-8902-AF5132FB4CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="130">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1179,6 +1179,27 @@
   </si>
   <si>
     <t>Product without Fortifier</t>
+  </si>
+  <si>
+    <t>EHM +  Fortifiers</t>
+  </si>
+  <si>
+    <t>EHM +  Fortifier + Modular</t>
+  </si>
+  <si>
+    <t>DHM +  Fortifiers</t>
+  </si>
+  <si>
+    <t>DHM +  Fortifier + Modular</t>
+  </si>
+  <si>
+    <t>Sterile Water + Fortifiers</t>
+  </si>
+  <si>
+    <t>EHM + DHM +  Fortifiers</t>
+  </si>
+  <si>
+    <t>EHM or DHM + Fortifier + Modular</t>
   </si>
 </sst>
 </file>
@@ -1749,7 +1770,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 42 
+              <c:v>0 OUT OF 49 
 PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
@@ -1845,7 +1866,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 42</c:v>
+                  <c:v>Failed or not yet done: 49</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Passed: 0</c:v>
@@ -3029,10 +3050,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W56"/>
+  <dimension ref="A1:W63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3058,13 +3079,13 @@
       <c r="D1" s="25"/>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1023), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2), "%")</f>
-        <v>0 OUT OF 42 
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1030), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1030))*100,2), "%")</f>
+        <v>0 OUT OF 49 
 PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 42</v>
+        <v>Failed or not yet done: 49</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
@@ -3083,11 +3104,11 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1023))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1030))*100,2)</f>
         <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1023))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1030))*100,2)</f>
         <v>0</v>
       </c>
     </row>
@@ -3344,7 +3365,7 @@
     <row r="28" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="33" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C28" s="30" t="b">
         <v>0</v>
@@ -3354,7 +3375,7 @@
     <row r="29" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="33" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="C29" s="30" t="b">
         <v>0</v>
@@ -3363,130 +3384,129 @@
     </row>
     <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1"/>
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="33" t="s">
+        <v>116</v>
+      </c>
+      <c r="C30" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D30" s="26"/>
+    </row>
+    <row r="31" spans="1:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="1"/>
+      <c r="B31" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="26"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="1"/>
+      <c r="B32" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D32" s="26"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1"/>
+      <c r="B33" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D33" s="26"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1"/>
+      <c r="B34" s="31" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D34" s="26"/>
+    </row>
+    <row r="35" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1"/>
+      <c r="B35" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1"/>
+      <c r="B36" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="C30" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D30" s="26"/>
-    </row>
-    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="1"/>
-      <c r="B31" s="31" t="s">
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1"/>
+      <c r="B37" s="31" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="1"/>
-      <c r="B32" s="31" t="s">
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1"/>
+      <c r="B38" s="31" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D32" s="26"/>
-    </row>
-    <row r="33" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="1"/>
-      <c r="B33" s="31" t="s">
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1"/>
+      <c r="B39" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="C39" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1"/>
+      <c r="B40" s="31" t="s">
         <v>121</v>
       </c>
-      <c r="C33" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D33" s="26"/>
-    </row>
-    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="31" t="s">
+      <c r="C40" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B41" s="31" t="s">
         <v>118</v>
       </c>
-      <c r="C34" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D34" s="26"/>
-    </row>
-    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+      <c r="C41" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B42" s="27" t="s">
         <v>82</v>
-      </c>
-      <c r="C35" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="1"/>
-      <c r="B36" s="27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C36" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B37" s="32" t="s">
-        <v>110</v>
-      </c>
-      <c r="C37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="1"/>
-      <c r="B38" s="32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C38" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B39" s="32" t="s">
-        <v>112</v>
-      </c>
-      <c r="C39" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="1"/>
-      <c r="B40" s="27" t="s">
-        <v>106</v>
-      </c>
-      <c r="C40" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A41" s="1"/>
-      <c r="B41" s="32" t="s">
-        <v>107</v>
-      </c>
-      <c r="C41" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="26"/>
-    </row>
-    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="1"/>
-      <c r="B42" s="32" t="s">
-        <v>108</v>
       </c>
       <c r="C42" s="30" t="b">
         <v>0</v>
@@ -3495,29 +3515,100 @@
     </row>
     <row r="43" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
-      <c r="B43" s="32" t="s">
+      <c r="B43" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D43" s="26"/>
+    </row>
+    <row r="44" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" s="32" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1"/>
+      <c r="B45" s="32" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C46" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="26"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="1"/>
+      <c r="B47" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="1"/>
+      <c r="B48" s="32" t="s">
+        <v>107</v>
+      </c>
+      <c r="C48" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="26"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="1"/>
+      <c r="B49" s="32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D49" s="26"/>
+    </row>
+    <row r="50" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="1"/>
+      <c r="B50" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="C43" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D43" s="26"/>
-    </row>
-    <row r="44" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="C50" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D50" s="26"/>
+    </row>
+    <row r="51" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C43">
+  <conditionalFormatting sqref="C2:C50">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
API-4980 receive ehm step 1
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2ADFEFA-1112-4082-BF66-A8E7F6F6D145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF41FBB5-4824-4532-83B4-395787121AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1206,6 +1206,15 @@
   </si>
   <si>
     <t>Print Collection Label UI Verification - Hard and Soft Stop</t>
+  </si>
+  <si>
+    <t>Receive Human Milk Step 1 UI Verification</t>
+  </si>
+  <si>
+    <t>Dispose</t>
+  </si>
+  <si>
+    <t>Dispose Bottle</t>
   </si>
 </sst>
 </file>
@@ -1596,7 +1605,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1726,6 +1735,9 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1776,7 +1788,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 43 
+              <c:v>0 OUT OF 45 
 PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
@@ -1872,7 +1884,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 43</c:v>
+                  <c:v>Failed or not yet done: 45</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Passed: 0</c:v>
@@ -3056,10 +3068,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W57"/>
+  <dimension ref="A1:W58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3087,13 +3099,13 @@
       </c>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1024), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1024))*100,2), "%")</f>
-        <v>0 OUT OF 43 
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1025), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1025))*100,2), "%")</f>
+        <v>0 OUT OF 45 
 PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 43</v>
+        <v>Failed or not yet done: 45</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
@@ -3112,11 +3124,11 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1024))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1025))*100,2)</f>
         <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1024))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1025))*100,2)</f>
         <v>0</v>
       </c>
     </row>
@@ -3371,49 +3383,49 @@
     <row r="28" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
       <c r="B28" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C28" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D28" s="26"/>
+    </row>
+    <row r="29" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="33" t="s">
         <v>122</v>
       </c>
-      <c r="C28" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="C29" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D29" s="26"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B30" s="33" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D29" s="26"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-      <c r="B30" s="33" t="s">
-        <v>117</v>
-      </c>
       <c r="C30" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="1"/>
       <c r="B31" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" s="26"/>
+    </row>
+    <row r="32" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="33" t="s">
         <v>119</v>
-      </c>
-      <c r="C31" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D31" s="26"/>
-    </row>
-    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-      <c r="B32" s="27" t="s">
-        <v>107</v>
       </c>
       <c r="C32" s="30" t="b">
         <v>0</v>
@@ -3422,8 +3434,8 @@
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
-      <c r="B33" s="31" t="s">
-        <v>109</v>
+      <c r="B33" s="27" t="s">
+        <v>107</v>
       </c>
       <c r="C33" s="30" t="b">
         <v>0</v>
@@ -3433,7 +3445,7 @@
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="1"/>
       <c r="B34" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C34" s="30" t="b">
         <v>0</v>
@@ -3443,121 +3455,142 @@
     <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="1"/>
       <c r="B35" s="31" t="s">
+        <v>111</v>
+      </c>
+      <c r="C35" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D35" s="26"/>
+    </row>
+    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="31" t="s">
         <v>113</v>
       </c>
-      <c r="C35" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D35" s="26"/>
-    </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="C36" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D36" s="26"/>
+    </row>
+    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B36" s="27" t="s">
+      <c r="B37" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C36" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D36" s="26"/>
-    </row>
-    <row r="37" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-      <c r="B37" s="27" t="s">
+      <c r="C37" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D37" s="26"/>
+    </row>
+    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="27" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D37" s="26"/>
-    </row>
-    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1" t="s">
+      <c r="C38" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D38" s="26"/>
+    </row>
+    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B38" s="32" t="s">
+      <c r="B39" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C38" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D38" s="26"/>
-    </row>
-    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-      <c r="B39" s="32" t="s">
+      <c r="C39" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D39" s="26"/>
+    </row>
+    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C39" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D39" s="26"/>
-    </row>
-    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="32" t="s">
+      <c r="C40" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D40" s="26"/>
+    </row>
+    <row r="41" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C40" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D40" s="26"/>
-    </row>
-    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-      <c r="B41" s="27" t="s">
+      <c r="C41" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D41" s="26"/>
+    </row>
+    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C41" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D41" s="26"/>
-    </row>
-    <row r="42" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-      <c r="B42" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="C42" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D42" s="26"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="1"/>
       <c r="B43" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C43" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D43" s="26"/>
     </row>
-    <row r="44" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C44" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C44" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D44" s="26"/>
-    </row>
-    <row r="45" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C45" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>127</v>
+      </c>
+      <c r="C46" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="26"/>
+    </row>
     <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C44">
+  <conditionalFormatting sqref="C2:C46">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
Fix pump date dropdown and next button in receive product
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jseroy\Desktop\Timeless\Important\Automation for peer review\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1AC401-1D21-427D-AC77-212BC9B6FA67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF226C2-499B-4BE9-8287-40A7EA79F1D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Result" sheetId="1" r:id="rId1"/>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="129">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1215,6 +1215,44 @@
   </si>
   <si>
     <t>Dispose Bottle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">• Scenario Error Testing - Previously Received Milk 
+     • Expected output: 
+         Hard Stop Message =  The container(s) have already been received: EHM00002I,EHM00002J 
+     • Actual Output: 
+         Hard Stop Message = The container(s) have already been received:  EHM00002I,EHM00002J
+• Scenario Error Testing - Previously Received MBMS 
+     • Expected output: 
+         Hard Stop Message = The container that you selected D031000153030001026410152601215081532 is a donor milk. 
+     • Actual Output: 
+         Hard Stop Message = The container that you selected D031000153030001026410152601215081532 is a donor milk.
+• Scenario Error Testing - Previously Received Product 
+     • Expected output: 
+         Hard Stop Message =  This container  FRM00002L  cannot be received back into inventory as it has been prepared with formula items. 
+     • Actual Output: 
+         Hard Stop Message =  This container  FRM00002L  cannot be received back into inventory as it has been prepared with formula items.
+• Scenario Error Testing - Random Barcode 
+     • Expected output: 
+         Hard Stop Message =  The container  123456  is not a valid container. 
+     • Actual Output: 
+         Hard Stop Message =  The container  123456  is not a valid container. 
+• Scenario Error Testing - Disposed Container 
+     • Expected output: 
+         Hard Stop Message =  The container that you selected  EHM00002I  has already been disposed. 
+     • Actual Output: 
+         Hard Stop Message =  The container that you selected  EHM00002I  has already been disposed.
+• Scenario Error Testing - Expired Container 
+     • Expected output: 
+         Hard Stop Message =  Expired Container 
+     • Actual Output: 
+         Hard Stop Message =  No expired bottle
+• Scenario Error Testing - Discharge Mother 
+     • Expected output: 
+         Hard Stop Message =  The guardian that you selected  is not active. 
+     • Actual Output: 
+         Hard Stop Message =  The guardian that you selected  is not active.
+</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1260,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -1670,7 +1708,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="44" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
@@ -1785,8 +1823,8 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 45 
-PERCENT = 0%</c:v>
+              <c:v>6 OUT OF 45 
+PERCENT = 13.33%</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1881,10 +1919,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 45</c:v>
+                  <c:v>Failed or not yet done: 39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Passed: 0</c:v>
+                  <c:v>Passed: 6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1896,10 +1934,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>86.67</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>13.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3071,17 +3109,17 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="27.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="3" max="3" width="9.109375" customWidth="1"/>
     <col min="4" max="4" width="163" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" customWidth="1"/>
-    <col min="22" max="22" width="21.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
+    <col min="22" max="22" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="29.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="24" t="s">
         <v>74</v>
       </c>
@@ -3097,19 +3135,19 @@
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
         <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1025), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1025))*100,2), "%")</f>
-        <v>0 OUT OF 45 
-PERCENT = 0%</v>
+        <v>6 OUT OF 45 
+PERCENT = 13.33%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 45</v>
+        <v>Failed or not yet done: 39</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
-        <v>Passed: 0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>Passed: 6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -3122,14 +3160,14 @@
       <c r="D2" s="26"/>
       <c r="V2">
         <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1025))*100,2)</f>
-        <v>100</v>
+        <v>86.67</v>
       </c>
       <c r="W2">
         <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1025))*100,2)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="27" t="s">
         <v>88</v>
@@ -3138,7 +3176,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="27" t="s">
         <v>90</v>
       </c>
@@ -3147,7 +3185,7 @@
       </c>
       <c r="D4" s="26"/>
     </row>
-    <row r="5" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="27" t="s">
         <v>89</v>
@@ -3157,7 +3195,7 @@
       </c>
       <c r="D5" s="26"/>
     </row>
-    <row r="6" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="27" t="s">
         <v>123</v>
@@ -3167,7 +3205,7 @@
       </c>
       <c r="D6" s="26"/>
     </row>
-    <row r="7" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>0</v>
       </c>
@@ -3178,7 +3216,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="27" t="s">
         <v>1</v>
@@ -3187,7 +3225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="27" t="s">
         <v>2</v>
@@ -3196,7 +3234,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="28" t="s">
         <v>91</v>
@@ -3205,7 +3243,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="29" t="s">
         <v>92</v>
@@ -3214,7 +3252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="29" t="s">
         <v>93</v>
@@ -3223,7 +3261,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="29" t="s">
         <v>94</v>
@@ -3232,7 +3270,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="29" t="s">
         <v>95</v>
@@ -3241,7 +3279,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>77</v>
       </c>
@@ -3253,7 +3291,7 @@
       </c>
       <c r="D15" s="26"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="29" t="s">
         <v>99</v>
@@ -3263,7 +3301,7 @@
       </c>
       <c r="D16" s="26"/>
     </row>
-    <row r="17" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="28" t="s">
         <v>96</v>
@@ -3273,7 +3311,7 @@
       </c>
       <c r="D17" s="26"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="29" t="s">
         <v>97</v>
@@ -3283,7 +3321,7 @@
       </c>
       <c r="D18" s="26"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>78</v>
       </c>
@@ -3291,11 +3329,11 @@
         <v>86</v>
       </c>
       <c r="C19" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="26"/>
     </row>
-    <row r="20" spans="1:4" ht="39" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="27" t="s">
         <v>124</v>
@@ -3305,7 +3343,7 @@
       </c>
       <c r="D20" s="26"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>79</v>
       </c>
@@ -3313,21 +3351,21 @@
         <v>87</v>
       </c>
       <c r="C21" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="26"/>
     </row>
-    <row r="22" spans="1:4" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="27.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="28" t="s">
         <v>100</v>
       </c>
       <c r="C22" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="26"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="29" t="s">
         <v>101</v>
@@ -3337,27 +3375,27 @@
       </c>
       <c r="D23" s="26"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="29" t="s">
         <v>102</v>
       </c>
       <c r="C24" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="26"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="29" t="s">
         <v>103</v>
       </c>
       <c r="C25" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="26"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
       <c r="B26" s="29" t="s">
         <v>104</v>
@@ -3367,7 +3405,7 @@
       </c>
       <c r="D26" s="26"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
       <c r="B27" s="29" t="s">
         <v>105</v>
@@ -3377,7 +3415,7 @@
       </c>
       <c r="D27" s="26"/>
     </row>
-    <row r="28" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="409.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1"/>
       <c r="B28" s="33" t="s">
         <v>125</v>
@@ -3385,9 +3423,11 @@
       <c r="C28" s="30" t="b">
         <v>0</v>
       </c>
-      <c r="D28" s="26"/>
-    </row>
-    <row r="29" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D28" s="26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="1"/>
       <c r="B29" s="33" t="s">
         <v>122</v>
@@ -3397,7 +3437,7 @@
       </c>
       <c r="D29" s="26"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>80</v>
       </c>
@@ -3409,7 +3449,7 @@
       </c>
       <c r="D30" s="26"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="1"/>
       <c r="B31" s="33" t="s">
         <v>117</v>
@@ -3419,7 +3459,7 @@
       </c>
       <c r="D31" s="26"/>
     </row>
-    <row r="32" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="1"/>
       <c r="B32" s="33" t="s">
         <v>119</v>
@@ -3429,7 +3469,7 @@
       </c>
       <c r="D32" s="26"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="1"/>
       <c r="B33" s="27" t="s">
         <v>107</v>
@@ -3439,7 +3479,7 @@
       </c>
       <c r="D33" s="26"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1"/>
       <c r="B34" s="31" t="s">
         <v>109</v>
@@ -3449,7 +3489,7 @@
       </c>
       <c r="D34" s="26"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="1"/>
       <c r="B35" s="31" t="s">
         <v>111</v>
@@ -3459,7 +3499,7 @@
       </c>
       <c r="D35" s="26"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1"/>
       <c r="B36" s="31" t="s">
         <v>113</v>
@@ -3469,7 +3509,7 @@
       </c>
       <c r="D36" s="26"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -3481,7 +3521,7 @@
       </c>
       <c r="D37" s="26"/>
     </row>
-    <row r="38" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1"/>
       <c r="B38" s="27" t="s">
         <v>106</v>
@@ -3491,7 +3531,7 @@
       </c>
       <c r="D38" s="26"/>
     </row>
-    <row r="39" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>83</v>
       </c>
@@ -3503,7 +3543,7 @@
       </c>
       <c r="D39" s="26"/>
     </row>
-    <row r="40" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="1"/>
       <c r="B40" s="32" t="s">
         <v>118</v>
@@ -3513,7 +3553,7 @@
       </c>
       <c r="D40" s="26"/>
     </row>
-    <row r="41" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="32" t="s">
         <v>120</v>
       </c>
@@ -3522,7 +3562,7 @@
       </c>
       <c r="D41" s="26"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1"/>
       <c r="B42" s="27" t="s">
         <v>108</v>
@@ -3532,7 +3572,7 @@
       </c>
       <c r="D42" s="26"/>
     </row>
-    <row r="43" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="1"/>
       <c r="B43" s="32" t="s">
         <v>110</v>
@@ -3542,7 +3582,7 @@
       </c>
       <c r="D43" s="26"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="1"/>
       <c r="B44" s="32" t="s">
         <v>112</v>
@@ -3552,7 +3592,7 @@
       </c>
       <c r="D44" s="26"/>
     </row>
-    <row r="45" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="1"/>
       <c r="B45" s="32" t="s">
         <v>114</v>
@@ -3562,7 +3602,7 @@
       </c>
       <c r="D45" s="26"/>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -3570,22 +3610,22 @@
         <v>127</v>
       </c>
       <c r="C46" s="30" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D46" s="26"/>
     </row>
-    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="27.6" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <conditionalFormatting sqref="C2:C46">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
@@ -3609,35 +3649,35 @@
       <selection activeCell="A22" sqref="A22:C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="46.28515625" customWidth="1"/>
-    <col min="3" max="3" width="59.5703125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="46.33203125" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="39" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="40"/>
       <c r="C1" s="40"/>
     </row>
-    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="42"/>
       <c r="C2" s="42"/>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="34" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -3648,7 +3688,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -3662,7 +3702,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -3676,7 +3716,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>15</v>
       </c>
@@ -3687,7 +3727,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -3698,7 +3738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -3709,7 +3749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -3723,7 +3763,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -3737,7 +3777,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
@@ -3751,28 +3791,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A13" s="39" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="40"/>
       <c r="C13" s="40"/>
     </row>
-    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="41" t="s">
         <v>33</v>
       </c>
       <c r="B14" s="42"/>
       <c r="C14" s="42"/>
     </row>
-    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="34" t="s">
         <v>34</v>
       </c>
       <c r="B15" s="35"/>
       <c r="C15" s="35"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>6</v>
       </c>
@@ -3783,7 +3823,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>9</v>
       </c>
@@ -3797,7 +3837,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -3811,7 +3851,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -3825,7 +3865,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>18</v>
       </c>
@@ -3839,7 +3879,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>21</v>
       </c>
@@ -3850,7 +3890,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>24</v>
       </c>
@@ -3864,7 +3904,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>27</v>
       </c>
@@ -3878,7 +3918,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -3889,7 +3929,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>51</v>
       </c>
@@ -3903,7 +3943,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>54</v>
       </c>
@@ -3917,28 +3957,28 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="36" t="s">
         <v>57</v>
       </c>
       <c r="B27" s="36"/>
       <c r="C27" s="36"/>
     </row>
-    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B28" s="7"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="37" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="38"/>
       <c r="C29" s="38"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>6</v>
       </c>
@@ -3949,7 +3989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>9</v>
       </c>
@@ -3960,7 +4000,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="13" t="s">
         <v>12</v>
       </c>
@@ -3971,7 +4011,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>15</v>
       </c>
@@ -3985,7 +4025,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>18</v>
       </c>
@@ -3999,7 +4039,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="57.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="10" t="s">
         <v>21</v>
       </c>
@@ -4013,7 +4053,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
@@ -4024,7 +4064,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="10" t="s">
         <v>27</v>
       </c>
@@ -4035,20 +4075,20 @@
         <v>73</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="20"/>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="23"/>
       <c r="C39" s="21"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B41" s="21"/>
       <c r="C41" s="23"/>
     </row>
@@ -4074,7 +4114,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4086,7 +4126,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4098,7 +4138,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4110,7 +4150,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Split Received RTU Product to Assigned Patient
</commit_message>
<xml_diff>
--- a/Assets/Excel/SmokeTestScenariosAndResults.xlsx
+++ b/Assets/Excel/SmokeTestScenariosAndResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Documents\UiPath\TMNP-Smoke-Testing-Automation\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4485F2E-9110-49CD-9ED0-0D531A372FAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCEBF06-F955-463E-996C-2D88E4EB368C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CD556FE-C62F-4787-89A0-8DF20AA637B2}"/>
   </bookViews>
@@ -193,7 +193,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="135">
   <si>
     <t>Manage Patient</t>
   </si>
@@ -1233,6 +1233,9 @@
   </si>
   <si>
     <t>Split Unreceived RTU Product to Assigned Patient</t>
+  </si>
+  <si>
+    <t>Split Received RTU Product to Assigned Patient</t>
   </si>
 </sst>
 </file>
@@ -1803,7 +1806,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>0 OUT OF 51 
+              <c:v>0 OUT OF 52 
 PERCENT = 0%</c:v>
             </c:pt>
           </c:strCache>
@@ -1899,7 +1902,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>Failed or not yet done: 51</c:v>
+                  <c:v>Failed or not yet done: 52</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Passed: 0</c:v>
@@ -3083,10 +3086,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82861F96-65CD-4331-A53A-0E92CB2941D8}">
-  <dimension ref="A1:W64"/>
+  <dimension ref="A1:W65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3114,13 +3117,13 @@
       </c>
       <c r="F1" s="1"/>
       <c r="T1" s="24" t="str">
-        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1031), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1031))*100,2), "%")</f>
-        <v>0 OUT OF 51 
+        <f>CONCATENATE("", COUNTIF($C:$C,TRUE)," OUT OF ", COUNTA($C2:$C1032), " ", CHAR(10), "PERCENT = ",ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1032))*100,2), "%")</f>
+        <v>0 OUT OF 52 
 PERCENT = 0%</v>
       </c>
       <c r="V1" t="str">
         <f>_xlfn.CONCAT("Failed or not yet done: ", COUNTIF($C:$C,FALSE))</f>
-        <v>Failed or not yet done: 51</v>
+        <v>Failed or not yet done: 52</v>
       </c>
       <c r="W1" t="str">
         <f>_xlfn.CONCAT("Passed: ", COUNTIF($C:$C,TRUE))</f>
@@ -3139,11 +3142,11 @@
       </c>
       <c r="D2" s="26"/>
       <c r="V2">
-        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1031))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,FALSE)/COUNTA($C2:$C1032))*100,2)</f>
         <v>100</v>
       </c>
       <c r="W2">
-        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1031))*100,2)</f>
+        <f>ROUND((COUNTIF($C:$C,TRUE)/COUNTA($C2:$C1032))*100,2)</f>
         <v>0</v>
       </c>
     </row>
@@ -3562,110 +3565,120 @@
     <row r="44" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="1"/>
       <c r="B44" s="32" t="s">
+        <v>134</v>
+      </c>
+      <c r="C44" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="45" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="1"/>
+      <c r="B45" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="C44" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D44" s="26"/>
-    </row>
-    <row r="45" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1" t="s">
+      <c r="C45" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D45" s="26"/>
+    </row>
+    <row r="46" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="B45" s="32" t="s">
+      <c r="B46" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="C45" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D45" s="26"/>
-    </row>
-    <row r="46" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-      <c r="B46" s="32" t="s">
+      <c r="C46" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D46" s="26"/>
+    </row>
+    <row r="47" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="1"/>
+      <c r="B47" s="32" t="s">
         <v>118</v>
       </c>
-      <c r="C46" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D46" s="26"/>
-    </row>
-    <row r="47" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="32" t="s">
+      <c r="C47" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D47" s="26"/>
+    </row>
+    <row r="48" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="C47" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D47" s="26"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-      <c r="B48" s="27" t="s">
+      <c r="C48" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D48" s="26"/>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="1"/>
+      <c r="B49" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C48" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D48" s="26"/>
-    </row>
-    <row r="49" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-      <c r="B49" s="32" t="s">
-        <v>110</v>
-      </c>
       <c r="C49" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D49" s="26"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="1"/>
       <c r="B50" s="32" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C50" s="30" t="b">
         <v>0</v>
       </c>
       <c r="D50" s="26"/>
     </row>
-    <row r="51" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="1"/>
       <c r="B51" s="32" t="s">
+        <v>112</v>
+      </c>
+      <c r="C51" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D51" s="26"/>
+    </row>
+    <row r="52" spans="1:4" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="1"/>
+      <c r="B52" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="C51" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D51" s="26"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="C52" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D52" s="26"/>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>126</v>
       </c>
-      <c r="B52" s="32" t="s">
+      <c r="B53" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="C52" s="30" t="b">
-        <v>0</v>
-      </c>
-      <c r="D52" s="26"/>
-    </row>
-    <row r="53" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="C53" s="30" t="b">
+        <v>0</v>
+      </c>
+      <c r="D53" s="26"/>
+    </row>
     <row r="54" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="56" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="57" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="58" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="59" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="60" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="1:4" ht="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="61" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="62" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="63" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="64" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <conditionalFormatting sqref="C2:C52">
+  <conditionalFormatting sqref="C2:C53">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="FALSE">
       <formula>NOT(ISERROR(SEARCH("FALSE",C2)))</formula>
     </cfRule>

</xml_diff>